<commit_message>
Changed: Pins.h, added camera stuff, added external libraries
added much stuff including external PID libraries, new camera.h and camera.cpp code and simplified drive_system.cpp so that I can I change the drive pins through Pins.h.
</commit_message>
<xml_diff>
--- a/Pinins for Arduino LW2024.xlsx
+++ b/Pinins for Arduino LW2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\23729\Documents\RCJA-Lightweight-Competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4220502E-3030-4713-85E3-983DB0C8D752}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83BB4FA-4E18-4AD7-804C-4F4D236F0110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" xr2:uid="{F81D8EB1-569A-4B72-8AFC-C74F347C21B0}"/>
   </bookViews>
@@ -679,7 +679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56ED041-E376-4570-BD48-C8084F43DEAB}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -825,26 +827,26 @@
       <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>80</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>23</v>
       </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated to 12 tssps on xlsx
</commit_message>
<xml_diff>
--- a/Pinins for Arduino LW2024.xlsx
+++ b/Pinins for Arduino LW2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\23729\Documents\RCJA-Lightweight-Competition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E83BB4FA-4E18-4AD7-804C-4F4D236F0110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E92CF49-A303-4FBA-B8FB-51FDC25D42B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="350" windowWidth="19420" windowHeight="10560" xr2:uid="{F81D8EB1-569A-4B72-8AFC-C74F347C21B0}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="90">
-  <si>
-    <t>Motor</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="78">
   <si>
     <t>Tssp</t>
   </si>
@@ -47,9 +44,6 @@
     <t>Light Sensor</t>
   </si>
   <si>
-    <t>Compass (BNO/IMU)</t>
-  </si>
-  <si>
     <t>Camera</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>D53</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>A0</t>
   </si>
   <si>
@@ -279,33 +270,6 @@
   </si>
   <si>
     <t>D0/RX</t>
-  </si>
-  <si>
-    <t>12 (2D, 1P)</t>
-  </si>
-  <si>
-    <t>2 (20,22)</t>
-  </si>
-  <si>
-    <t>2 (RX/TX)</t>
-  </si>
-  <si>
-    <t>16 (Digi)</t>
-  </si>
-  <si>
-    <t>16 (Ana)</t>
-  </si>
-  <si>
-    <t>Pinins</t>
-  </si>
-  <si>
-    <t>Initialization</t>
-  </si>
-  <si>
-    <t>What</t>
-  </si>
-  <si>
-    <t>Number of pins</t>
   </si>
 </sst>
 </file>
@@ -677,572 +641,494 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56ED041-E376-4570-BD48-C8084F43DEAB}">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:B70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" t="s">
-        <v>86</v>
-      </c>
-      <c r="I3" t="s">
-        <v>88</v>
-      </c>
-      <c r="J3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" t="s">
-        <v>63</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" t="s">
-        <v>63</v>
-      </c>
-      <c r="I5" t="s">
-        <v>0</v>
-      </c>
-      <c r="J5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="B16" t="s">
         <v>2</v>
-      </c>
-      <c r="J6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I7" t="s">
-        <v>3</v>
-      </c>
-      <c r="J7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>51</v>
-      </c>
-      <c r="B43" t="s">
-        <v>1</v>
+        <v>49</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45" t="s">
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" t="s">
-        <v>1</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B56" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B61" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B62" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B66" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B69" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B70" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>